<commit_message>
update templates for release other and issuetrak
</commit_message>
<xml_diff>
--- a/templates/skill-grading-template-test.xlsx
+++ b/templates/skill-grading-template-test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\career-training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\career-training\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Doe, John" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
   <si>
     <t>Career Development</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Jane Doe</t>
-  </si>
-  <si>
-    <t># of completed software project major/minor releases</t>
   </si>
   <si>
     <t>Earned</t>
@@ -388,6 +385,12 @@
   </si>
   <si>
     <t>ISTQB Agile Tester (CTFL-AT)</t>
+  </si>
+  <si>
+    <t># of completed OTHER software project major/minor releases</t>
+  </si>
+  <si>
+    <t># of completed ISSUETRAK software project major/minor releases</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -584,6 +583,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,7 +641,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color theme="0"/>
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
@@ -656,7 +659,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="0"/>
+        <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
@@ -856,9 +859,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A13:F24" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A13:F24"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="0"/>
-    <tableColumn id="2" name="Novice" dataDxfId="5"/>
-    <tableColumn id="3" name="Advanced Beginner" dataDxfId="4"/>
+    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="5"/>
+    <tableColumn id="2" name="Novice" dataDxfId="4"/>
+    <tableColumn id="3" name="Advanced Beginner" dataDxfId="3"/>
     <tableColumn id="4" name="Competent"/>
     <tableColumn id="5" name="Proficient"/>
     <tableColumn id="6" name="Expert"/>
@@ -868,12 +871,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:F24" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:F24" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A13:F24"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="2"/>
+    <tableColumn id="1" name="Software Engineering Discipline" dataDxfId="1"/>
     <tableColumn id="2" name="Novice"/>
-    <tableColumn id="3" name="Advanced Beginner" dataDxfId="1"/>
+    <tableColumn id="3" name="Advanced Beginner" dataDxfId="0"/>
     <tableColumn id="4" name="Competent"/>
     <tableColumn id="5" name="Proficient"/>
     <tableColumn id="6" name="Expert"/>
@@ -1147,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1232,13 +1235,13 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -1266,11 +1269,11 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="5"/>
       <c r="H14" s="7" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1278,13 +1281,13 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1295,9 +1298,9 @@
         <v>17</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32" t="s">
-        <v>83</v>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>16</v>
@@ -1310,8 +1313,8 @@
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>83</v>
+      <c r="B17" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1321,7 +1324,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1330,13 +1333,13 @@
         <v>74</v>
       </c>
       <c r="I18" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="K18" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1344,7 +1347,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1355,16 +1358,16 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -1373,7 +1376,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1381,51 +1384,51 @@
         <v>33</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="D23" s="32" t="s">
-        <v>83</v>
+      <c r="D23" s="30" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>83</v>
+      <c r="B24" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="H26" s="31"/>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="H27" s="31"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H28" s="31"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H29" s="31"/>
+      <c r="H29" s="29"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H30" s="31"/>
+      <c r="H30" s="29"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H31" s="31"/>
+      <c r="H31" s="29"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H32" s="31"/>
+      <c r="H32" s="29"/>
     </row>
     <row r="33" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H33" s="31"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H34" s="31"/>
+      <c r="H34" s="29"/>
     </row>
     <row r="35" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H35" s="31"/>
+      <c r="H35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1443,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1484,7 +1487,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1529,13 +1532,13 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -1564,13 +1567,13 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="H14" s="7" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="I14" s="5">
         <v>15</v>
@@ -1578,17 +1581,17 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="32" t="s">
-        <v>83</v>
+      <c r="C15" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="H15" s="7" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="I15" s="5">
         <v>5</v>
@@ -1599,10 +1602,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="32"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="32" t="s">
-        <v>83</v>
+      <c r="E16" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="F16" s="24"/>
       <c r="H16" s="7" t="s">
@@ -1617,8 +1620,8 @@
         <v>18</v>
       </c>
       <c r="B17" s="24"/>
-      <c r="C17" s="32" t="s">
-        <v>83</v>
+      <c r="C17" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1631,21 +1634,21 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="24"/>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="32" t="s">
         <v>74</v>
       </c>
       <c r="I18" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="K18" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1654,13 +1657,13 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="H19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I19" s="20">
         <v>42005</v>
@@ -1673,12 +1676,12 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="H20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I20" s="20">
         <v>42156</v>
@@ -1686,12 +1689,12 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="24"/>
       <c r="D21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
@@ -1701,8 +1704,8 @@
         <v>32</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="32" t="s">
-        <v>83</v>
+      <c r="C22" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -1714,8 +1717,8 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="32" t="s">
-        <v>83</v>
+      <c r="D23" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1727,8 +1730,8 @@
       <c r="B24" s="24"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="32" t="s">
-        <v>83</v>
+      <c r="E24" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="F24" s="24"/>
     </row>
@@ -1761,7 +1764,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -1774,7 +1777,7 @@
         <v>73</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1815,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>30</v>
@@ -1820,13 +1823,13 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>